<commit_message>
Updated pages "AES cipher internals in Excel", "DES cipher internals in Excel", "Poor feedback from readers".
</commit_message>
<xml_diff>
--- a/des-cipher-internals-in-excel/des-cipher-internals.xlsx
+++ b/des-cipher-internals-in-excel/des-cipher-internals.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="105" windowWidth="23835" windowHeight="10110"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11610"/>
   </bookViews>
   <sheets>
     <sheet name="DES" sheetId="6" r:id="rId1"/>
     <sheet name="S-boxes" sheetId="5" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -341,9 +341,6 @@
     <t>XOR left (no swap)</t>
   </si>
   <si>
-    <t>http://nayuki.eigenstate.org/page/des-cipher-internals-in-excel</t>
-  </si>
-  <si>
     <t>Extract bits</t>
   </si>
   <si>
@@ -355,11 +352,14 @@
   <si>
     <t>DES Cipher Internals</t>
   </si>
+  <si>
+    <t>http://www.nayuki.io/page/des-cipher-internals-in-excel</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -711,6 +711,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -758,7 +761,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -793,7 +796,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1018,7 +1021,7 @@
   <sheetData>
     <row r="1" spans="1:130" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="27" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B1" s="27"/>
       <c r="C1" s="27"/>
@@ -1219,7 +1222,7 @@
       <c r="BL2" s="26"/>
       <c r="BM2" s="26"/>
       <c r="BN2" s="26" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="BO2" s="26"/>
       <c r="BP2" s="26"/>
@@ -3134,7 +3137,7 @@
       <c r="DX11" s="4"/>
       <c r="DY11" s="4"/>
       <c r="DZ11" s="24" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="12" spans="1:130" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3558,7 +3561,7 @@
       <c r="DX12" s="4"/>
       <c r="DY12" s="4"/>
       <c r="DZ12" s="24" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="13" spans="1:130" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -4926,7 +4929,7 @@
       <c r="DX17" s="4"/>
       <c r="DY17" s="4"/>
       <c r="DZ17" s="24" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="18" spans="1:130" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -5350,7 +5353,7 @@
       <c r="DX18" s="4"/>
       <c r="DY18" s="4"/>
       <c r="DZ18" s="24" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="19" spans="1:130" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -6718,7 +6721,7 @@
       <c r="DX23" s="4"/>
       <c r="DY23" s="4"/>
       <c r="DZ23" s="24" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="24" spans="1:130" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -7142,7 +7145,7 @@
       <c r="DX24" s="4"/>
       <c r="DY24" s="4"/>
       <c r="DZ24" s="24" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="25" spans="1:130" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -8510,7 +8513,7 @@
       <c r="DX29" s="4"/>
       <c r="DY29" s="4"/>
       <c r="DZ29" s="24" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="30" spans="1:130" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -8934,7 +8937,7 @@
       <c r="DX30" s="4"/>
       <c r="DY30" s="4"/>
       <c r="DZ30" s="24" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="31" spans="1:130" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -10302,7 +10305,7 @@
       <c r="DX35" s="4"/>
       <c r="DY35" s="4"/>
       <c r="DZ35" s="24" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="36" spans="1:130" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -10726,7 +10729,7 @@
       <c r="DX36" s="4"/>
       <c r="DY36" s="4"/>
       <c r="DZ36" s="24" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="37" spans="1:130" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -12094,7 +12097,7 @@
       <c r="DX41" s="4"/>
       <c r="DY41" s="4"/>
       <c r="DZ41" s="24" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="42" spans="1:130" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -12518,7 +12521,7 @@
       <c r="DX42" s="4"/>
       <c r="DY42" s="4"/>
       <c r="DZ42" s="24" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="43" spans="1:130" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -13886,7 +13889,7 @@
       <c r="DX47" s="4"/>
       <c r="DY47" s="4"/>
       <c r="DZ47" s="24" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="48" spans="1:130" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -14310,7 +14313,7 @@
       <c r="DX48" s="4"/>
       <c r="DY48" s="4"/>
       <c r="DZ48" s="24" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="49" spans="1:130" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -15678,7 +15681,7 @@
       <c r="DX53" s="4"/>
       <c r="DY53" s="4"/>
       <c r="DZ53" s="24" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="54" spans="1:130" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -16102,7 +16105,7 @@
       <c r="DX54" s="4"/>
       <c r="DY54" s="4"/>
       <c r="DZ54" s="24" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="55" spans="1:130" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -17470,7 +17473,7 @@
       <c r="DX59" s="4"/>
       <c r="DY59" s="4"/>
       <c r="DZ59" s="24" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="60" spans="1:130" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -17894,7 +17897,7 @@
       <c r="DX60" s="4"/>
       <c r="DY60" s="4"/>
       <c r="DZ60" s="24" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="61" spans="1:130" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -19262,7 +19265,7 @@
       <c r="DX65" s="4"/>
       <c r="DY65" s="4"/>
       <c r="DZ65" s="24" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="66" spans="1:130" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -19686,7 +19689,7 @@
       <c r="DX66" s="4"/>
       <c r="DY66" s="4"/>
       <c r="DZ66" s="24" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="67" spans="1:130" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -21054,7 +21057,7 @@
       <c r="DX71" s="4"/>
       <c r="DY71" s="4"/>
       <c r="DZ71" s="24" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="72" spans="1:130" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -21478,7 +21481,7 @@
       <c r="DX72" s="4"/>
       <c r="DY72" s="4"/>
       <c r="DZ72" s="24" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="73" spans="1:130" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -22846,7 +22849,7 @@
       <c r="DX77" s="4"/>
       <c r="DY77" s="4"/>
       <c r="DZ77" s="24" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="78" spans="1:130" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -23270,7 +23273,7 @@
       <c r="DX78" s="4"/>
       <c r="DY78" s="4"/>
       <c r="DZ78" s="24" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="79" spans="1:130" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -24638,7 +24641,7 @@
       <c r="DX83" s="4"/>
       <c r="DY83" s="4"/>
       <c r="DZ83" s="24" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="84" spans="1:130" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -25062,7 +25065,7 @@
       <c r="DX84" s="4"/>
       <c r="DY84" s="4"/>
       <c r="DZ84" s="24" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="85" spans="1:130" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -26430,7 +26433,7 @@
       <c r="DX89" s="4"/>
       <c r="DY89" s="4"/>
       <c r="DZ89" s="24" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="90" spans="1:130" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -26854,7 +26857,7 @@
       <c r="DX90" s="4"/>
       <c r="DY90" s="4"/>
       <c r="DZ90" s="24" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="91" spans="1:130" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -28222,7 +28225,7 @@
       <c r="DX95" s="4"/>
       <c r="DY95" s="4"/>
       <c r="DZ95" s="24" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="96" spans="1:130" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -28646,7 +28649,7 @@
       <c r="DX96" s="4"/>
       <c r="DY96" s="4"/>
       <c r="DZ96" s="24" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="97" spans="1:130" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -30014,7 +30017,7 @@
       <c r="DX101" s="4"/>
       <c r="DY101" s="4"/>
       <c r="DZ101" s="24" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="102" spans="1:130" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -30438,7 +30441,7 @@
       <c r="DX102" s="4"/>
       <c r="DY102" s="4"/>
       <c r="DZ102" s="24" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="103" spans="1:130" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>